<commit_message>
added files from week 9
</commit_message>
<xml_diff>
--- a/jiao-research/jiao-group-gantt-seanlai.xlsx
+++ b/jiao-research/jiao-group-gantt-seanlai.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seanlai/Projects/school/jiao-research/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5380DD4-7DD8-4149-B6F1-C05E07E913AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E11A0FD-07BD-CC4F-9A27-1A67AB2537D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -785,23 +785,23 @@
     <xf numFmtId="0" fontId="13" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="13" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="13" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="13" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="165" fontId="13" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="13" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="13" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="13" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="13" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1363,7 +1363,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -1390,44 +1390,44 @@
       <c r="E1" s="19"/>
       <c r="G1" s="17"/>
       <c r="H1" s="20"/>
-      <c r="I1" s="79"/>
-      <c r="J1" s="79"/>
-      <c r="K1" s="79"/>
-      <c r="L1" s="79"/>
-      <c r="M1" s="79"/>
-      <c r="N1" s="79"/>
-      <c r="O1" s="79"/>
-      <c r="P1" s="79"/>
-      <c r="Q1" s="79"/>
-      <c r="R1" s="79"/>
-      <c r="S1" s="79"/>
-      <c r="T1" s="79"/>
-      <c r="U1" s="79"/>
-      <c r="V1" s="79"/>
-      <c r="W1" s="79"/>
-      <c r="X1" s="79"/>
-      <c r="Y1" s="79"/>
-      <c r="Z1" s="79"/>
+      <c r="I1" s="74"/>
+      <c r="J1" s="74"/>
+      <c r="K1" s="74"/>
+      <c r="L1" s="74"/>
+      <c r="M1" s="74"/>
+      <c r="N1" s="74"/>
+      <c r="O1" s="74"/>
+      <c r="P1" s="74"/>
+      <c r="Q1" s="74"/>
+      <c r="R1" s="74"/>
+      <c r="S1" s="74"/>
+      <c r="T1" s="74"/>
+      <c r="U1" s="74"/>
+      <c r="V1" s="74"/>
+      <c r="W1" s="74"/>
+      <c r="X1" s="74"/>
+      <c r="Y1" s="74"/>
+      <c r="Z1" s="74"/>
     </row>
     <row r="2" spans="1:63" ht="19.5" customHeight="1">
       <c r="B2" s="21"/>
       <c r="C2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="74">
+      <c r="D2" s="78">
         <v>43922</v>
       </c>
-      <c r="E2" s="75"/>
+      <c r="E2" s="79"/>
     </row>
     <row r="3" spans="1:63" ht="19.5" customHeight="1">
       <c r="B3" s="21"/>
       <c r="C3" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="74">
+      <c r="D3" s="78">
         <v>43994</v>
       </c>
-      <c r="E3" s="75"/>
+      <c r="E3" s="79"/>
     </row>
     <row r="4" spans="1:63" ht="19.5" customHeight="1">
       <c r="C4" s="22" t="s">
@@ -1436,86 +1436,86 @@
       <c r="D4" s="23">
         <v>8</v>
       </c>
-      <c r="H4" s="76">
+      <c r="H4" s="75">
         <f>H5</f>
         <v>43969</v>
       </c>
-      <c r="I4" s="77"/>
-      <c r="J4" s="77"/>
-      <c r="K4" s="77"/>
-      <c r="L4" s="77"/>
-      <c r="M4" s="77"/>
-      <c r="N4" s="78"/>
-      <c r="O4" s="76">
+      <c r="I4" s="76"/>
+      <c r="J4" s="76"/>
+      <c r="K4" s="76"/>
+      <c r="L4" s="76"/>
+      <c r="M4" s="76"/>
+      <c r="N4" s="77"/>
+      <c r="O4" s="75">
         <f>O5</f>
         <v>43976</v>
       </c>
-      <c r="P4" s="77"/>
-      <c r="Q4" s="77"/>
-      <c r="R4" s="77"/>
-      <c r="S4" s="77"/>
-      <c r="T4" s="77"/>
-      <c r="U4" s="78"/>
-      <c r="V4" s="76">
+      <c r="P4" s="76"/>
+      <c r="Q4" s="76"/>
+      <c r="R4" s="76"/>
+      <c r="S4" s="76"/>
+      <c r="T4" s="76"/>
+      <c r="U4" s="77"/>
+      <c r="V4" s="75">
         <f>V5</f>
         <v>43983</v>
       </c>
-      <c r="W4" s="77"/>
-      <c r="X4" s="77"/>
-      <c r="Y4" s="77"/>
-      <c r="Z4" s="77"/>
-      <c r="AA4" s="77"/>
-      <c r="AB4" s="78"/>
-      <c r="AC4" s="76">
+      <c r="W4" s="76"/>
+      <c r="X4" s="76"/>
+      <c r="Y4" s="76"/>
+      <c r="Z4" s="76"/>
+      <c r="AA4" s="76"/>
+      <c r="AB4" s="77"/>
+      <c r="AC4" s="75">
         <f>AC5</f>
         <v>43990</v>
       </c>
-      <c r="AD4" s="77"/>
-      <c r="AE4" s="77"/>
-      <c r="AF4" s="77"/>
-      <c r="AG4" s="77"/>
-      <c r="AH4" s="77"/>
-      <c r="AI4" s="78"/>
-      <c r="AJ4" s="76">
+      <c r="AD4" s="76"/>
+      <c r="AE4" s="76"/>
+      <c r="AF4" s="76"/>
+      <c r="AG4" s="76"/>
+      <c r="AH4" s="76"/>
+      <c r="AI4" s="77"/>
+      <c r="AJ4" s="75">
         <f>AJ5</f>
         <v>43997</v>
       </c>
-      <c r="AK4" s="77"/>
-      <c r="AL4" s="77"/>
-      <c r="AM4" s="77"/>
-      <c r="AN4" s="77"/>
-      <c r="AO4" s="77"/>
-      <c r="AP4" s="78"/>
-      <c r="AQ4" s="76">
+      <c r="AK4" s="76"/>
+      <c r="AL4" s="76"/>
+      <c r="AM4" s="76"/>
+      <c r="AN4" s="76"/>
+      <c r="AO4" s="76"/>
+      <c r="AP4" s="77"/>
+      <c r="AQ4" s="75">
         <f>AQ5</f>
         <v>44004</v>
       </c>
-      <c r="AR4" s="77"/>
-      <c r="AS4" s="77"/>
-      <c r="AT4" s="77"/>
-      <c r="AU4" s="77"/>
-      <c r="AV4" s="77"/>
-      <c r="AW4" s="78"/>
-      <c r="AX4" s="76">
+      <c r="AR4" s="76"/>
+      <c r="AS4" s="76"/>
+      <c r="AT4" s="76"/>
+      <c r="AU4" s="76"/>
+      <c r="AV4" s="76"/>
+      <c r="AW4" s="77"/>
+      <c r="AX4" s="75">
         <f>AX5</f>
         <v>44011</v>
       </c>
-      <c r="AY4" s="77"/>
-      <c r="AZ4" s="77"/>
-      <c r="BA4" s="77"/>
-      <c r="BB4" s="77"/>
-      <c r="BC4" s="77"/>
-      <c r="BD4" s="78"/>
-      <c r="BE4" s="76">
+      <c r="AY4" s="76"/>
+      <c r="AZ4" s="76"/>
+      <c r="BA4" s="76"/>
+      <c r="BB4" s="76"/>
+      <c r="BC4" s="76"/>
+      <c r="BD4" s="77"/>
+      <c r="BE4" s="75">
         <f>BE5</f>
         <v>44018</v>
       </c>
-      <c r="BF4" s="77"/>
-      <c r="BG4" s="77"/>
-      <c r="BH4" s="77"/>
-      <c r="BI4" s="77"/>
-      <c r="BJ4" s="77"/>
-      <c r="BK4" s="78"/>
+      <c r="BF4" s="76"/>
+      <c r="BG4" s="76"/>
+      <c r="BH4" s="76"/>
+      <c r="BI4" s="76"/>
+      <c r="BJ4" s="76"/>
+      <c r="BK4" s="77"/>
     </row>
     <row r="5" spans="1:63">
       <c r="A5" s="22"/>
@@ -2207,7 +2207,9 @@
       <c r="B10" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="44"/>
+      <c r="C10" s="44">
+        <v>1</v>
+      </c>
       <c r="D10" s="45">
         <v>43969</v>
       </c>
@@ -2281,7 +2283,9 @@
       <c r="B11" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="44"/>
+      <c r="C11" s="44">
+        <v>1</v>
+      </c>
       <c r="D11" s="45">
         <v>43972</v>
       </c>
@@ -4441,17 +4445,17 @@
   </sheetData>
   <autoFilter ref="B1:E4" xr:uid="{07A7420B-EC04-D349-8A81-AEBC5B1CBC8D}"/>
   <mergeCells count="11">
-    <mergeCell ref="I1:Z1"/>
-    <mergeCell ref="AJ4:AP4"/>
-    <mergeCell ref="AQ4:AW4"/>
-    <mergeCell ref="AX4:BD4"/>
-    <mergeCell ref="BE4:BK4"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="H4:N4"/>
     <mergeCell ref="O4:U4"/>
     <mergeCell ref="V4:AB4"/>
     <mergeCell ref="AC4:AI4"/>
     <mergeCell ref="D3:E3"/>
+    <mergeCell ref="I1:Z1"/>
+    <mergeCell ref="AJ4:AP4"/>
+    <mergeCell ref="AQ4:AW4"/>
+    <mergeCell ref="AX4:BD4"/>
+    <mergeCell ref="BE4:BK4"/>
   </mergeCells>
   <conditionalFormatting sqref="C7:C27">
     <cfRule type="dataBar" priority="12">

</xml_diff>